<commit_message>
Validate double Quote fixed
</commit_message>
<xml_diff>
--- a/wwwroot/ExcelTest.xlsx
+++ b/wwwroot/ExcelTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmess\source\repos\FileConverter\wwwroot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\K88677\source\repos\FileConverter\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69C5B40A-56BA-404A-934A-0D750F535212}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE115CB-5539-4959-895E-2E49DE825CC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -59,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="172">
   <si>
     <t>3 Self-Promotion</t>
   </si>
@@ -572,6 +569,9 @@
   </si>
   <si>
     <t>ww</t>
+  </si>
+  <si>
+    <t>3 Self,Promotion</t>
   </si>
 </sst>
 </file>
@@ -579,16 +579,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="10">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="0.00%_);[Red]\(0.00%\)"/>
-    <numFmt numFmtId="169" formatCode="0%_);[Red]\(0%\)"/>
-    <numFmt numFmtId="170" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="171" formatCode="0.00%_);[Red]\(0.00%\)"/>
+    <numFmt numFmtId="172" formatCode="0%_);[Red]\(0%\)"/>
+    <numFmt numFmtId="173" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -951,24 +951,24 @@
     <xf numFmtId="37" fontId="2" fillId="3" borderId="1" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="5" fontId="8" fillId="0" borderId="2">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyBorder="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="5" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3"/>
     <xf numFmtId="4" fontId="8" fillId="5" borderId="3">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="4" fontId="8" fillId="6" borderId="3"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="4"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="4"/>
     <xf numFmtId="37" fontId="5" fillId="7" borderId="2" applyBorder="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -984,8 +984,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0">
       <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="7"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="8"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="7"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="8"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
@@ -993,8 +993,8 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="169" fontId="13" fillId="9" borderId="10"/>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="10" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="172" fontId="13" fillId="9" borderId="10"/>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="10" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1007,11 +1007,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1023,12 +1023,12 @@
     <xf numFmtId="0" fontId="21" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="21" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="21" fillId="12" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="21" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="21" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="12" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="21" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="37">
     <cellStyle name="amount" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1647,7 +1647,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1"/>
@@ -3384,7 +3384,7 @@
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>171</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>143</v>
@@ -3404,7 +3404,7 @@
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>0</v>
+        <v>171</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>143</v>

</xml_diff>